<commit_message>
added comments and fixed it from RR-3 to RR-5
</commit_message>
<xml_diff>
--- a/RoundRobinTesting.xlsx
+++ b/RoundRobinTesting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brycecallender/Desktop/OperatingSystemProjects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bryce\Desktop\OperatingSystemProjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B8D9C25-270A-D245-9CB6-65C371150397}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4634A45B-9EDF-49AB-AF5C-8B66E67AA2A9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" xr2:uid="{3BB9B1C9-75B4-0342-96C2-A3EE28745992}"/>
+    <workbookView xWindow="4290" yWindow="4290" windowWidth="28800" windowHeight="15435" xr2:uid="{3BB9B1C9-75B4-0342-96C2-A3EE28745992}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="13">
   <si>
     <t>Round Robin (2)</t>
   </si>
@@ -60,10 +60,10 @@
     <t xml:space="preserve">Finished </t>
   </si>
   <si>
-    <t>Round Robin (3)</t>
-  </si>
-  <si>
     <t xml:space="preserve">JOB </t>
+  </si>
+  <si>
+    <t>Round Robin (5)</t>
   </si>
 </sst>
 </file>
@@ -417,13 +417,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C14AC30-0BC8-CB41-BE69-21FEE971803C}">
   <dimension ref="A1:AC13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,7 +431,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -520,7 +520,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -609,7 +609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -698,7 +698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -787,7 +787,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -813,14 +813,14 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="R7">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -832,7 +832,7 @@
         <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
@@ -859,31 +859,10 @@
         <v>8</v>
       </c>
       <c r="O8" t="s">
-        <v>12</v>
-      </c>
-      <c r="P8" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>8</v>
-      </c>
-      <c r="R8" t="s">
-        <v>8</v>
-      </c>
-      <c r="S8" t="s">
-        <v>8</v>
-      </c>
-      <c r="T8" t="s">
-        <v>8</v>
-      </c>
-      <c r="U8" t="s">
-        <v>8</v>
-      </c>
-      <c r="V8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -918,40 +897,19 @@
         <v>3</v>
       </c>
       <c r="L9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M9">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="O9">
         <v>2</v>
       </c>
-      <c r="P9">
-        <v>3</v>
-      </c>
-      <c r="Q9">
-        <v>5</v>
-      </c>
-      <c r="R9">
-        <v>2</v>
-      </c>
-      <c r="S9">
-        <v>3</v>
-      </c>
-      <c r="T9">
-        <v>5</v>
-      </c>
-      <c r="U9">
-        <v>2</v>
-      </c>
-      <c r="V9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -962,64 +920,43 @@
         <v>9</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>7</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>9</v>
-      </c>
       <c r="I10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M10">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="N10">
         <v>0</v>
       </c>
       <c r="O10">
-        <v>9</v>
-      </c>
-      <c r="P10">
-        <v>1</v>
-      </c>
-      <c r="Q10">
-        <v>3</v>
-      </c>
-      <c r="R10">
-        <v>6</v>
-      </c>
-      <c r="S10">
         <v>0</v>
       </c>
-      <c r="T10">
-        <v>0</v>
-      </c>
-      <c r="U10">
-        <v>3</v>
-      </c>
-      <c r="V10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1030,90 +967,69 @@
         <v>5</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E11">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F11">
-        <v>9</v>
-      </c>
-      <c r="G11">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>6</v>
       </c>
       <c r="H11">
-        <v>15</v>
-      </c>
-      <c r="I11">
-        <v>18</v>
+        <v>24</v>
+      </c>
+      <c r="I11" t="s">
+        <v>6</v>
       </c>
       <c r="J11">
-        <v>21</v>
-      </c>
-      <c r="K11">
-        <v>24</v>
-      </c>
-      <c r="L11" t="s">
-        <v>6</v>
+        <v>31</v>
+      </c>
+      <c r="K11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11">
+        <v>41</v>
       </c>
       <c r="M11">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="N11" t="s">
         <v>6</v>
       </c>
-      <c r="O11">
-        <v>32</v>
-      </c>
-      <c r="P11">
-        <v>35</v>
-      </c>
-      <c r="Q11">
-        <v>38</v>
-      </c>
-      <c r="R11">
-        <v>41</v>
-      </c>
-      <c r="S11" t="s">
-        <v>6</v>
-      </c>
-      <c r="T11" t="s">
-        <v>6</v>
-      </c>
-      <c r="U11">
+      <c r="O11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>19</v>
+      </c>
+      <c r="I12">
+        <v>26</v>
+      </c>
+      <c r="K12">
+        <v>36</v>
+      </c>
+      <c r="N12">
         <v>48</v>
       </c>
-      <c r="V11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12">
-        <v>4</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="L12">
-        <v>25</v>
-      </c>
-      <c r="N12">
-        <v>29</v>
-      </c>
-      <c r="S12">
-        <v>42</v>
-      </c>
-      <c r="T12">
-        <v>45</v>
-      </c>
-      <c r="V12">
+      <c r="O12">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>

</xml_diff>